<commit_message>
Updated sponsor gallery view template; update attribution
Added a new compiled PHP template for the sponsor gallery block. Updated image attribution in sigcon-landing-cards-flexrow to conditionally display the license only if present. Updated sigdoc-schedule.xlsx with new content.
</commit_message>
<xml_diff>
--- a/sigdoc-schedule.xlsx
+++ b/sigdoc-schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/calindgr/Documents/Local Sites/sigdocconference/app/public/wp-content/themes/theme-sigcon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A87CC13-9850-D445-93AC-C11E6BD5330E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A898F2FA-6B0C-5A48-9342-6753F5F06B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38300" yWindow="500" windowWidth="25480" windowHeight="28300" activeTab="1" xr2:uid="{73101ED4-5EDA-8B46-BBBC-F6B89C9A8C85}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="36000" windowHeight="22520" activeTab="1" xr2:uid="{73101ED4-5EDA-8B46-BBBC-F6B89C9A8C85}"/>
   </bookViews>
   <sheets>
     <sheet name="sigdoc-schedule-2024" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1408" uniqueCount="610">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1408" uniqueCount="609">
   <si>
     <t>date</t>
   </si>
@@ -1205,9 +1205,6 @@
     <t>Margaret Hsiao</t>
   </si>
   <si>
-    <t>Designing Power: A Comparative Analysis of the White House Websites Under Presidents Biden and Trump</t>
-  </si>
-  <si>
     <t>Heather Turner</t>
   </si>
   <si>
@@ -1268,9 +1265,6 @@
     <t>Graduate Research Roundtables</t>
   </si>
   <si>
-    <t>Ashely Hardin, Manushri Pandaya, Chenxing Xie, Emily Gresbrink, Rebekka Anderson, and Carlos Evia</t>
-  </si>
-  <si>
     <t>Cara Haderlie, Jamal-Jared Alexander and Avery Edenfield</t>
   </si>
   <si>
@@ -1367,9 +1361,6 @@
     <t>Beyond Usability: Experience Architecture as a Framework for Ethical UX Design</t>
   </si>
   <si>
-    <t>Mckinley Green</t>
-  </si>
-  <si>
     <t>Visibility of Gender Pronouns on Campus Learning Management Systems: A UX study</t>
   </si>
   <si>
@@ -1535,12 +1526,6 @@
     <t>Linguistic greenscapes: The design of dispensary exterior signage</t>
   </si>
   <si>
-    <t>Anirban Ray, Edzordzi Agbozo, Ian Weaver and Yeqing Kong</t>
-  </si>
-  <si>
-    <t>Rethinking Persuasive Design in Crisis: Cultural Dimensions of COVID-19 mHealth Technologies</t>
-  </si>
-  <si>
     <t>The Promise of Solidarity: Addressing Lateral Violence in Institutional Critique</t>
   </si>
   <si>
@@ -1562,9 +1547,6 @@
     <t>High Tech Teaching Trajectory: An Analysis of Graduate to Undergraduate Mentorship in the Professional Writing Classroom</t>
   </si>
   <si>
-    <t>Mckinley Green, Chakrika Veeramoothoo, Nicole Ciulla and Jeremy Rosselot-Merritt</t>
-  </si>
-  <si>
     <t>Navigating academic and non-academic careers: The shared experiences of a PhD cohort community</t>
   </si>
   <si>
@@ -1851,6 +1833,21 @@
   </si>
   <si>
     <t>An informal, conversational session for graduate researchers to share ideas, exchange contacts, or simply mingle. No need to prepare formal presentations or talks.</t>
+  </si>
+  <si>
+    <t>Designing Power: A Comparative Analysis of the White House Websites</t>
+  </si>
+  <si>
+    <t>McKinley Green, Chakrika Veeramoothoo, Nicole Ciulla and Jeremy Rosselot-Merritt</t>
+  </si>
+  <si>
+    <t>Ashley Hardin, Manushri Pandaya, Chenxing Xie, Emily Gresbrink, Rebekka Andersen, and Carlos Evia</t>
+  </si>
+  <si>
+    <t>Gabriel Aguilar</t>
+  </si>
+  <si>
+    <t>The Links Between Artificial Intelligence and Scams on Latines: Preparing Technical Communicators for the Future of AI Scams</t>
   </si>
 </sst>
 </file>
@@ -6613,8 +6610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B47D8858-3BEC-FE4D-BA46-291391952D5A}">
   <dimension ref="A1:N119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H119" sqref="H119"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H113" sqref="H113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6678,25 +6675,25 @@
         <v>45939</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
       <c r="I2" s="3" t="b">
         <v>1</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="K2" s="3" t="b">
         <v>0</v>
@@ -6710,16 +6707,16 @@
         <v>45954</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>188</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>563</v>
+        <v>557</v>
       </c>
       <c r="I3" s="3" t="b">
         <v>0</v>
@@ -6739,13 +6736,13 @@
         <v>390</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>391</v>
@@ -6771,7 +6768,7 @@
         <v>29</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>347</v>
@@ -6800,7 +6797,7 @@
         <v>29</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>387</v>
@@ -6829,7 +6826,7 @@
         <v>29</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>349</v>
@@ -6861,7 +6858,7 @@
         <v>29</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>35</v>
@@ -6893,7 +6890,7 @@
         <v>29</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>41</v>
@@ -6925,13 +6922,13 @@
         <v>29</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>393</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>394</v>
+        <v>604</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>392</v>
@@ -6957,7 +6954,7 @@
         <v>29</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>353</v>
@@ -6966,7 +6963,7 @@
         <v>354</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="I11" s="3" t="b">
         <v>0</v>
@@ -6989,7 +6986,7 @@
         <v>29</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>355</v>
@@ -6998,7 +6995,7 @@
         <v>356</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="I12" s="3" t="b">
         <v>0</v>
@@ -7021,7 +7018,7 @@
         <v>29</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>357</v>
@@ -7030,7 +7027,7 @@
         <v>358</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="I13" s="3" t="b">
         <v>0</v>
@@ -7053,7 +7050,7 @@
         <v>29</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>359</v>
@@ -7062,7 +7059,7 @@
         <v>360</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="I14" s="3" t="b">
         <v>0</v>
@@ -7085,7 +7082,7 @@
         <v>29</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>361</v>
@@ -7094,7 +7091,7 @@
         <v>362</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="I15" s="3" t="b">
         <v>0</v>
@@ -7117,7 +7114,7 @@
         <v>29</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>363</v>
@@ -7126,7 +7123,7 @@
         <v>364</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="I16" s="3" t="b">
         <v>0</v>
@@ -7149,16 +7146,16 @@
         <v>29</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
       <c r="F17" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>398</v>
-      </c>
       <c r="H17" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="I17" s="3" t="b">
         <v>0</v>
@@ -7181,7 +7178,7 @@
         <v>112</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>366</v>
@@ -7210,7 +7207,7 @@
         <v>112</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>368</v>
@@ -7239,7 +7236,7 @@
         <v>112</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>370</v>
@@ -7271,7 +7268,7 @@
         <v>112</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>372</v>
@@ -7303,13 +7300,13 @@
         <v>112</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="F22" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="G22" s="2" t="s">
         <v>399</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>400</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>357</v>
@@ -7335,7 +7332,7 @@
         <v>112</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>374</v>
@@ -7344,7 +7341,7 @@
         <v>375</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="I23" s="3" t="b">
         <v>0</v>
@@ -7367,7 +7364,7 @@
         <v>112</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>376</v>
@@ -7376,7 +7373,7 @@
         <v>377</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="I24" s="3" t="b">
         <v>0</v>
@@ -7399,7 +7396,7 @@
         <v>112</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>378</v>
@@ -7408,7 +7405,7 @@
         <v>379</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="I25" s="3" t="b">
         <v>0</v>
@@ -7431,16 +7428,16 @@
         <v>112</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="F26" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="G26" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="H26" s="3" t="s">
         <v>402</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>403</v>
       </c>
       <c r="I26" s="3" t="b">
         <v>0</v>
@@ -7463,7 +7460,7 @@
         <v>112</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>380</v>
@@ -7472,7 +7469,7 @@
         <v>381</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I27" s="3" t="b">
         <v>0</v>
@@ -7495,7 +7492,7 @@
         <v>112</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>382</v>
@@ -7504,7 +7501,7 @@
         <v>383</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I28" s="3" t="b">
         <v>0</v>
@@ -7527,7 +7524,7 @@
         <v>112</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>283</v>
@@ -7536,7 +7533,7 @@
         <v>384</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I29" s="3" t="b">
         <v>0</v>
@@ -7559,16 +7556,16 @@
         <v>112</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
       <c r="F30" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="G30" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="H30" s="3" t="s">
         <v>405</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>406</v>
       </c>
       <c r="I30" s="3" t="b">
         <v>0</v>
@@ -7585,19 +7582,19 @@
         <v>45954</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>534</v>
+        <v>528</v>
       </c>
       <c r="E31" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="G31" s="2" t="s">
         <v>407</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>409</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>408</v>
       </c>
       <c r="I31" s="3" t="b">
         <v>0</v>
@@ -7609,7 +7606,7 @@
         <v>1</v>
       </c>
       <c r="N31" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.15">
@@ -7617,19 +7614,19 @@
         <v>45954</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>557</v>
+        <v>551</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
       <c r="I32" s="3" t="b">
         <v>0</v>
@@ -7646,19 +7643,19 @@
         <v>45954</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>557</v>
+        <v>551</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
       <c r="I33" s="3" t="b">
         <v>0</v>
@@ -7675,19 +7672,19 @@
         <v>45954</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>557</v>
+        <v>551</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>541</v>
+        <v>535</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
       <c r="I34" s="3" t="b">
         <v>0</v>
@@ -7704,19 +7701,19 @@
         <v>45954</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>557</v>
+        <v>551</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>544</v>
+        <v>538</v>
       </c>
       <c r="I35" s="3" t="b">
         <v>0</v>
@@ -7733,19 +7730,19 @@
         <v>45954</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>557</v>
+        <v>551</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>545</v>
+        <v>539</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>546</v>
+        <v>540</v>
       </c>
       <c r="I36" s="3" t="b">
         <v>0</v>
@@ -7762,19 +7759,19 @@
         <v>45954</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>557</v>
+        <v>551</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>547</v>
+        <v>541</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>548</v>
+        <v>542</v>
       </c>
       <c r="I37" s="3" t="b">
         <v>0</v>
@@ -7791,19 +7788,19 @@
         <v>45954</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>557</v>
+        <v>551</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>549</v>
+        <v>543</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="I38" s="3" t="b">
         <v>0</v>
@@ -7820,19 +7817,19 @@
         <v>45954</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>557</v>
+        <v>551</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>552</v>
+        <v>546</v>
       </c>
       <c r="I39" s="3" t="b">
         <v>0</v>
@@ -7849,19 +7846,19 @@
         <v>45954</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>557</v>
+        <v>551</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>554</v>
+        <v>548</v>
       </c>
       <c r="I40" s="3" t="b">
         <v>0</v>
@@ -7878,19 +7875,19 @@
         <v>45954</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>557</v>
+        <v>551</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>556</v>
+        <v>550</v>
       </c>
       <c r="I41" s="3" t="b">
         <v>0</v>
@@ -7907,19 +7904,19 @@
         <v>45954</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>569</v>
+        <v>563</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
       <c r="I42" s="3" t="b">
         <v>0</v>
@@ -7936,19 +7933,19 @@
         <v>45954</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>570</v>
+        <v>564</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>586</v>
+        <v>580</v>
       </c>
       <c r="I43" s="3" t="b">
         <v>0</v>
@@ -7965,19 +7962,19 @@
         <v>45954</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>218</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>587</v>
+        <v>581</v>
       </c>
       <c r="I44" s="3" t="b">
         <v>0</v>
@@ -7994,19 +7991,19 @@
         <v>45954</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>571</v>
+        <v>565</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>588</v>
+        <v>582</v>
       </c>
       <c r="I45" s="3" t="b">
         <v>0</v>
@@ -8023,19 +8020,19 @@
         <v>45954</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>572</v>
+        <v>566</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
       <c r="I46" s="3" t="b">
         <v>0</v>
@@ -8052,19 +8049,19 @@
         <v>45954</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>590</v>
+        <v>584</v>
       </c>
       <c r="I47" s="3" t="b">
         <v>0</v>
@@ -8081,19 +8078,19 @@
         <v>45954</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>573</v>
+        <v>567</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>591</v>
+        <v>585</v>
       </c>
       <c r="I48" s="3" t="b">
         <v>0</v>
@@ -8110,19 +8107,19 @@
         <v>45954</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>574</v>
+        <v>568</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>592</v>
+        <v>586</v>
       </c>
       <c r="I49" s="3" t="b">
         <v>0</v>
@@ -8139,19 +8136,19 @@
         <v>45954</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>575</v>
+        <v>569</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>593</v>
+        <v>587</v>
       </c>
       <c r="I50" s="3" t="b">
         <v>0</v>
@@ -8168,19 +8165,19 @@
         <v>45954</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>594</v>
+        <v>588</v>
       </c>
       <c r="I51" s="3" t="b">
         <v>0</v>
@@ -8197,19 +8194,19 @@
         <v>45954</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>595</v>
+        <v>589</v>
       </c>
       <c r="I52" s="3" t="b">
         <v>0</v>
@@ -8226,19 +8223,19 @@
         <v>45954</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>211</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>596</v>
+        <v>590</v>
       </c>
       <c r="I53" s="3" t="b">
         <v>0</v>
@@ -8255,19 +8252,19 @@
         <v>45954</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
       <c r="I54" s="3" t="b">
         <v>0</v>
@@ -8284,19 +8281,19 @@
         <v>45954</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
       <c r="I55" s="3" t="b">
         <v>0</v>
@@ -8313,19 +8310,19 @@
         <v>45954</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>599</v>
+        <v>593</v>
       </c>
       <c r="I56" s="3" t="b">
         <v>0</v>
@@ -8342,19 +8339,19 @@
         <v>45954</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>600</v>
+        <v>594</v>
       </c>
       <c r="I57" s="3" t="b">
         <v>0</v>
@@ -8371,19 +8368,19 @@
         <v>45954</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>582</v>
+        <v>576</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
       <c r="I58" s="3" t="b">
         <v>0</v>
@@ -8400,19 +8397,19 @@
         <v>45954</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
       <c r="I59" s="3" t="b">
         <v>0</v>
@@ -8429,19 +8426,19 @@
         <v>45954</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>584</v>
+        <v>578</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="I60" s="3" t="b">
         <v>0</v>
@@ -8458,19 +8455,19 @@
         <v>45954</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>66</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="I61" s="3" t="b">
         <v>0</v>
@@ -8493,10 +8490,10 @@
         <v>342</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G62" s="2"/>
       <c r="I62" s="3" t="b">
@@ -8517,16 +8514,16 @@
         <v>111</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
       <c r="F63" s="6" t="s">
-        <v>609</v>
+        <v>603</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>608</v>
+        <v>602</v>
       </c>
       <c r="I63" s="3" t="b">
         <v>0</v>
@@ -8543,19 +8540,19 @@
         <v>45954</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>24</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>566</v>
+        <v>560</v>
       </c>
       <c r="I64" s="3" t="b">
         <v>0</v>
@@ -8572,19 +8569,19 @@
         <v>45954</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
       <c r="F65" t="s">
-        <v>568</v>
+        <v>562</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>567</v>
+        <v>561</v>
       </c>
       <c r="I65" s="3" t="b">
         <v>0</v>
@@ -8601,16 +8598,16 @@
         <v>45954</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>184</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
       <c r="F66" t="s">
-        <v>565</v>
+        <v>559</v>
       </c>
       <c r="G66" s="2"/>
       <c r="I66" s="3" t="b">
@@ -8620,7 +8617,7 @@
         <v>1</v>
       </c>
       <c r="L66" s="3" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
       <c r="M66" s="3" t="b">
         <v>0</v>
@@ -8631,17 +8628,17 @@
         <v>45955</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>188</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="F67" s="2"/>
       <c r="G67" s="3" t="s">
-        <v>563</v>
+        <v>557</v>
       </c>
       <c r="I67" s="3" t="b">
         <v>0</v>
@@ -8661,14 +8658,14 @@
         <v>389</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
       <c r="F68" s="2"/>
       <c r="G68" s="2" t="s">
-        <v>564</v>
+        <v>558</v>
       </c>
       <c r="I68" s="3" t="b">
         <v>0</v>
@@ -8691,10 +8688,10 @@
         <v>147</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>415</v>
+        <v>606</v>
       </c>
       <c r="G69" s="2" t="s">
         <v>348</v>
@@ -8720,13 +8717,13 @@
         <v>147</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="I70" s="3" t="b">
         <v>0</v>
@@ -8749,13 +8746,13 @@
         <v>147</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="H71" s="3" t="s">
         <v>162</v>
@@ -8781,13 +8778,13 @@
         <v>147</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="H72" s="3" t="s">
         <v>162</v>
@@ -8813,13 +8810,13 @@
         <v>147</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="H73" s="3" t="s">
         <v>162</v>
@@ -8845,16 +8842,16 @@
         <v>147</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="I74" s="3" t="b">
         <v>0</v>
@@ -8877,16 +8874,16 @@
         <v>147</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="I75" s="3" t="b">
         <v>0</v>
@@ -8909,16 +8906,16 @@
         <v>147</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="H76" s="3" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="I76" s="3" t="b">
         <v>0</v>
@@ -8941,16 +8938,16 @@
         <v>147</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="F77" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="H77" s="3" t="s">
         <v>430</v>
-      </c>
-      <c r="G77" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="H77" s="3" t="s">
-        <v>432</v>
       </c>
       <c r="I77" s="3" t="b">
         <v>0</v>
@@ -8973,13 +8970,13 @@
         <v>147</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>392</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="H78" s="3" t="s">
         <v>273</v>
@@ -9005,13 +9002,13 @@
         <v>147</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="H79" s="3" t="s">
         <v>273</v>
@@ -9037,13 +9034,13 @@
         <v>147</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="H80" s="3" t="s">
         <v>273</v>
@@ -9069,13 +9066,13 @@
         <v>147</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="H81" s="3" t="s">
         <v>273</v>
@@ -9101,13 +9098,13 @@
         <v>386</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="I82" s="3" t="b">
         <v>0</v>
@@ -9130,13 +9127,13 @@
         <v>386</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="I83" s="3" t="b">
         <v>0</v>
@@ -9159,13 +9156,13 @@
         <v>386</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="H84" s="3" t="s">
         <v>245</v>
@@ -9191,13 +9188,13 @@
         <v>386</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="H85" s="3" t="s">
         <v>245</v>
@@ -9223,13 +9220,13 @@
         <v>386</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>448</v>
+        <v>395</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="H86" s="3" t="s">
         <v>245</v>
@@ -9255,13 +9252,13 @@
         <v>386</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="H87" s="3" t="s">
         <v>245</v>
@@ -9287,13 +9284,13 @@
         <v>386</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="H88" s="3" t="s">
         <v>376</v>
@@ -9319,13 +9316,13 @@
         <v>386</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="H89" s="3" t="s">
         <v>376</v>
@@ -9351,13 +9348,13 @@
         <v>386</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="F90" s="2" t="s">
         <v>320</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="H90" s="3" t="s">
         <v>376</v>
@@ -9383,13 +9380,13 @@
         <v>386</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="G91" s="2" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="H91" s="3" t="s">
         <v>376</v>
@@ -9415,16 +9412,16 @@
         <v>386</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="G92" s="2" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="H92" s="3" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="I92" s="3" t="b">
         <v>0</v>
@@ -9447,16 +9444,16 @@
         <v>386</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="H93" s="3" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="I93" s="3" t="b">
         <v>0</v>
@@ -9479,16 +9476,16 @@
         <v>386</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="G94" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="H94" s="3" t="s">
         <v>464</v>
-      </c>
-      <c r="H94" s="3" t="s">
-        <v>467</v>
       </c>
       <c r="I94" s="3" t="b">
         <v>0</v>
@@ -9511,16 +9508,16 @@
         <v>386</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="H95" s="3" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="I95" s="3" t="b">
         <v>0</v>
@@ -9537,19 +9534,19 @@
         <v>45955</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="I96" s="3" t="b">
         <v>0</v>
@@ -9561,7 +9558,7 @@
         <v>1</v>
       </c>
       <c r="N96" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.15">
@@ -9569,19 +9566,19 @@
         <v>45955</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="C97" s="3" t="s">
         <v>228</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="G97" s="2" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="I97" s="3" t="b">
         <v>0</v>
@@ -9598,19 +9595,19 @@
         <v>45955</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="C98" s="3" t="s">
         <v>228</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="G98" s="2" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="I98" s="3" t="b">
         <v>0</v>
@@ -9627,22 +9624,22 @@
         <v>45955</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="C99" s="3" t="s">
         <v>228</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="G99" s="2" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="H99" s="3" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="I99" s="3" t="b">
         <v>0</v>
@@ -9659,22 +9656,22 @@
         <v>45955</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="C100" s="3" t="s">
         <v>228</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="G100" s="2" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="H100" s="3" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="I100" s="3" t="b">
         <v>0</v>
@@ -9691,22 +9688,22 @@
         <v>45955</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="C101" s="3" t="s">
         <v>228</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="G101" s="2" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="H101" s="3" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="I101" s="3" t="b">
         <v>0</v>
@@ -9723,19 +9720,19 @@
         <v>45955</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="C102" s="3" t="s">
         <v>228</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="G102" s="2" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="H102" s="3" t="s">
         <v>117</v>
@@ -9755,19 +9752,19 @@
         <v>45955</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="C103" s="3" t="s">
         <v>228</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="G103" s="2" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="H103" s="3" t="s">
         <v>117</v>
@@ -9787,19 +9784,19 @@
         <v>45955</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="C104" s="3" t="s">
         <v>228</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="G104" s="2" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="H104" s="3" t="s">
         <v>117</v>
@@ -9819,19 +9816,19 @@
         <v>45955</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="C105" s="3" t="s">
         <v>228</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="G105" s="2" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="H105" s="3" t="s">
         <v>361</v>
@@ -9851,19 +9848,19 @@
         <v>45955</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="C106" s="3" t="s">
         <v>228</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="G106" s="2" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="H106" s="3" t="s">
         <v>361</v>
@@ -9883,19 +9880,19 @@
         <v>45955</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="C107" s="3" t="s">
         <v>228</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="G107" s="2" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="H107" s="3" t="s">
         <v>361</v>
@@ -9915,19 +9912,19 @@
         <v>45955</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="C108" s="3" t="s">
         <v>228</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="G108" s="2" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="I108" s="3" t="b">
         <v>0</v>
@@ -9944,19 +9941,19 @@
         <v>45955</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="C109" s="3" t="s">
         <v>228</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="G109" s="2" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="I109" s="3" t="b">
         <v>0</v>
@@ -9973,22 +9970,22 @@
         <v>45955</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="C110" s="3" t="s">
         <v>228</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="G110" s="2" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="H110" s="3" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="I110" s="3" t="b">
         <v>0</v>
@@ -10005,22 +10002,22 @@
         <v>45955</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="C111" s="3" t="s">
         <v>228</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="G111" s="2" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="H111" s="3" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="I111" s="3" t="b">
         <v>0</v>
@@ -10037,22 +10034,22 @@
         <v>45955</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="C112" s="3" t="s">
         <v>228</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="G112" s="2" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="H112" s="3" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="I112" s="3" t="b">
         <v>0</v>
@@ -10069,22 +10066,22 @@
         <v>45955</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="C113" s="3" t="s">
         <v>228</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>504</v>
+        <v>607</v>
       </c>
       <c r="G113" s="2" t="s">
-        <v>505</v>
+        <v>608</v>
       </c>
       <c r="H113" s="3" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="I113" s="3" t="b">
         <v>0</v>
@@ -10101,22 +10098,22 @@
         <v>45955</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="C114" s="3" t="s">
         <v>228</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="F114" s="2" t="s">
         <v>142</v>
       </c>
       <c r="G114" s="2" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="H114" s="2" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
       <c r="I114" s="3" t="b">
         <v>0</v>
@@ -10133,22 +10130,22 @@
         <v>45955</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="C115" s="3" t="s">
         <v>228</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="G115" s="2" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="H115" s="2" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
       <c r="I115" s="3" t="b">
         <v>0</v>
@@ -10165,22 +10162,22 @@
         <v>45955</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="C116" s="3" t="s">
         <v>228</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="F116" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="G116" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="H116" s="2" t="s">
         <v>509</v>
-      </c>
-      <c r="G116" s="2" t="s">
-        <v>510</v>
-      </c>
-      <c r="H116" s="2" t="s">
-        <v>515</v>
       </c>
       <c r="I116" s="3" t="b">
         <v>0</v>
@@ -10197,22 +10194,22 @@
         <v>45955</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="C117" s="3" t="s">
         <v>228</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="G117" s="2" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="H117" s="2" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
       <c r="I117" s="3" t="b">
         <v>0</v>
@@ -10229,19 +10226,19 @@
         <v>45955</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="C118" s="3" t="s">
         <v>228</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>513</v>
+        <v>605</v>
       </c>
       <c r="G118" s="2" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
       <c r="I118" s="3" t="b">
         <v>0</v>
@@ -10258,16 +10255,16 @@
         <v>45955</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
       <c r="F119" s="3" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
   </sheetData>

</xml_diff>